<commit_message>
updated maps with broodstock and chipps fish
</commit_message>
<xml_diff>
--- a/DeltaSmelt/data/Other_DS_Catch_2023.xlsx
+++ b/DeltaSmelt/data/Other_DS_Catch_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/omr_report_2023/DeltaSmelt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{787BD35E-2524-42B2-8B59-E6A0F1DBE280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{132FB442-DE21-4469-8CDC-640D403A33E8}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{787BD35E-2524-42B2-8B59-E6A0F1DBE280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91731C29-E089-4B28-9E35-A17FDAF341E6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{8F64CD41-F4EE-4058-8FB9-5486A67AD111}"/>
+    <workbookView xWindow="-23865" yWindow="3105" windowWidth="21600" windowHeight="11385" xr2:uid="{8F64CD41-F4EE-4058-8FB9-5486A67AD111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="27">
   <si>
     <t>Broodstock</t>
   </si>
@@ -114,13 +114,16 @@
   </si>
   <si>
     <t>VIE-LRA</t>
+  </si>
+  <si>
+    <t>SB018M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +155,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,8 +175,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -229,11 +244,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6DADC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -270,6 +305,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -285,6 +326,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -584,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD8A7C8-5596-4343-BF11-B766880EA5BD}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,11 +1108,11 @@
       <c r="B23" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>20</v>
+      <c r="C23" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E23" s="13">
         <v>90</v>
@@ -1077,7 +1122,14 @@
       </c>
       <c r="S23" s="5"/>
     </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>